<commit_message>
add images from list product
</commit_message>
<xml_diff>
--- a/frontend-admin/public/excel/AddProduct.xlsx
+++ b/frontend-admin/public/excel/AddProduct.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399A0483-0886-461F-B2AA-85ABC7D7FB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E26784-4889-40E5-BCC2-422FF613D140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F772D34D-6B2B-4FBA-8460-C2E2B8A3CB04}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>61a0a817f4c63405f41a5cb6 - Souvenir</t>
+  </si>
+  <si>
+    <t>Images</t>
   </si>
 </sst>
 </file>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFAED57-6927-4B19-8ABA-3C4F0EABD32A}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,11 +622,11 @@
     <col min="8" max="8" width="39.42578125" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="42.28515625" customWidth="1"/>
-    <col min="11" max="11" width="39.7109375" customWidth="1"/>
-    <col min="12" max="12" width="146.140625" customWidth="1"/>
+    <col min="11" max="12" width="39.7109375" customWidth="1"/>
+    <col min="13" max="13" width="146.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -658,10 +661,13 @@
         <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="9"/>
@@ -673,9 +679,10 @@
       <c r="I2" s="10"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="9"/>
@@ -684,9 +691,9 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="I3" s="5"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="9"/>
@@ -695,9 +702,9 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="I4" s="5"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9"/>
@@ -705,9 +712,9 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
@@ -716,7 +723,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="I6" s="5"/>
-      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>